<commit_message>
Added Store test cases
</commit_message>
<xml_diff>
--- a/UserData.xlsx
+++ b/UserData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="96">
   <si>
     <t>testuser1</t>
   </si>
@@ -646,7 +646,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I6" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,7 +1045,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>